<commit_message>
pylinting done after function addition to store op in excel
</commit_message>
<xml_diff>
--- a/Implementation/Outputs.xlsx
+++ b/Implementation/Outputs.xlsx
@@ -484,7 +484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -973,72 +973,141 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>99004351</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>Sem</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="6" t="n">
         <v>52</v>
       </c>
-      <c r="E8" t="n">
-        <v>65</v>
-      </c>
-      <c r="F8" t="n">
-        <v>39</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="E8" s="6" t="n">
+        <v>65</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>39</v>
+      </c>
+      <c r="G8" s="6" t="n">
         <v>87</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="6" t="n">
         <v>43</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="6" t="n">
         <v>55</v>
       </c>
-      <c r="J8" t="n">
-        <v>65</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="J8" s="6" t="n">
+        <v>65</v>
+      </c>
+      <c r="K8" s="6" t="n">
         <v>99</v>
       </c>
-      <c r="L8" t="n">
-        <v>91</v>
-      </c>
-      <c r="M8" t="n">
+      <c r="L8" s="6" t="n">
+        <v>91</v>
+      </c>
+      <c r="M8" s="6" t="n">
         <v>64</v>
       </c>
-      <c r="N8" t="n">
+      <c r="N8" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="O8" t="n">
+      <c r="O8" s="6" t="n">
         <v>79</v>
       </c>
-      <c r="P8" t="n">
+      <c r="P8" s="6" t="n">
         <v>86</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8" s="6" t="n">
         <v>44</v>
       </c>
-      <c r="R8" t="n">
+      <c r="R8" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="S8" t="n">
+      <c r="S8" s="6" t="n">
         <v>98</v>
       </c>
-      <c r="T8" t="n">
+      <c r="T8" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="U8" t="n">
-        <v>91</v>
+      <c r="U8" s="6" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>99004354</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sem</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>82</v>
+      </c>
+      <c r="D9" t="n">
+        <v>49</v>
+      </c>
+      <c r="E9" t="n">
+        <v>45</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" t="n">
+        <v>24</v>
+      </c>
+      <c r="I9" t="n">
+        <v>93</v>
+      </c>
+      <c r="J9" t="n">
+        <v>52</v>
+      </c>
+      <c r="K9" t="n">
+        <v>65</v>
+      </c>
+      <c r="L9" t="n">
+        <v>39</v>
+      </c>
+      <c r="M9" t="n">
+        <v>87</v>
+      </c>
+      <c r="N9" t="n">
+        <v>43</v>
+      </c>
+      <c r="O9" t="n">
+        <v>55</v>
+      </c>
+      <c r="P9" t="n">
+        <v>93</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>93</v>
+      </c>
+      <c r="R9" t="n">
+        <v>52</v>
+      </c>
+      <c r="S9" t="n">
+        <v>65</v>
+      </c>
+      <c r="T9" t="n">
+        <v>39</v>
+      </c>
+      <c r="U9" t="n">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
file restructured and options too
</commit_message>
<xml_diff>
--- a/Implementation/Outputs.xlsx
+++ b/Implementation/Outputs.xlsx
@@ -484,14 +484,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C301" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="A301" activeCellId="0" sqref="A301"/>
+      <selection pane="bottomRight" activeCell="C318" activeCellId="0" sqref="C318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.62890625" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -1286,7 +1286,7 @@
         </is>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="13.8" customHeight="1" s="7">
       <c r="A12" s="6" t="inlineStr">
         <is>
           <t>99004351</t>
@@ -1355,7 +1355,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="13.8" customHeight="1" s="7">
       <c r="A13" s="6" t="inlineStr">
         <is>
           <t>99004362</t>
@@ -1462,7 +1462,7 @@
         </is>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="13.8" customHeight="1" s="7">
       <c r="A14" s="6" t="inlineStr">
         <is>
           <t>99004351</t>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="13.8" customHeight="1" s="7">
       <c r="A15" s="6" t="inlineStr">
         <is>
           <t>99004362</t>
@@ -1676,7 +1676,7 @@
         </is>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="13.8" customHeight="1" s="7">
       <c r="A16" s="6" t="inlineStr">
         <is>
           <t>99004351</t>
@@ -1783,7 +1783,7 @@
         </is>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="13.8" customHeight="1" s="7">
       <c r="A17" s="6" t="inlineStr">
         <is>
           <t>99004360</t>
@@ -1890,7 +1890,7 @@
         </is>
       </c>
     </row>
-    <row r="18">
+    <row r="18" ht="13.8" customHeight="1" s="7">
       <c r="A18" s="6" t="inlineStr">
         <is>
           <t>99004351</t>
@@ -1998,72 +1998,431 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>99004359</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Sem</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>45</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>6</v>
-      </c>
-      <c r="F19" t="n">
-        <v>82</v>
-      </c>
-      <c r="G19" t="n">
-        <v>49</v>
-      </c>
-      <c r="H19" t="n">
-        <v>93</v>
-      </c>
-      <c r="I19" t="n">
-        <v>91</v>
-      </c>
-      <c r="J19" t="n">
-        <v>87</v>
-      </c>
-      <c r="K19" t="n">
-        <v>52</v>
-      </c>
-      <c r="L19" t="n">
-        <v>65</v>
-      </c>
-      <c r="M19" t="n">
-        <v>39</v>
-      </c>
-      <c r="N19" t="n">
-        <v>87</v>
-      </c>
-      <c r="O19" t="n">
-        <v>43</v>
-      </c>
-      <c r="P19" t="n">
-        <v>93</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>99</v>
-      </c>
-      <c r="R19" t="n">
-        <v>91</v>
-      </c>
-      <c r="S19" t="n">
-        <v>39</v>
-      </c>
-      <c r="T19" t="n">
-        <v>0</v>
-      </c>
-      <c r="U19" t="n">
-        <v>43</v>
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>99004352</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="C19" s="6" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="D19" s="6" t="inlineStr">
+        <is>
+          <t>algorithm</t>
+        </is>
+      </c>
+      <c r="E19" s="6" t="inlineStr">
+        <is>
+          <t>dbms</t>
+        </is>
+      </c>
+      <c r="F19" s="6" t="inlineStr">
+        <is>
+          <t>data st</t>
+        </is>
+      </c>
+      <c r="G19" s="6" t="inlineStr">
+        <is>
+          <t>php</t>
+        </is>
+      </c>
+      <c r="H19" s="6" t="inlineStr">
+        <is>
+          <t>selenum</t>
+        </is>
+      </c>
+      <c r="I19" s="6" t="inlineStr">
+        <is>
+          <t>hadoop</t>
+        </is>
+      </c>
+      <c r="J19" s="6" t="inlineStr">
+        <is>
+          <t>spark</t>
+        </is>
+      </c>
+      <c r="K19" s="6" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="L19" s="6" t="inlineStr">
+        <is>
+          <t>algorithm</t>
+        </is>
+      </c>
+      <c r="M19" s="6" t="inlineStr">
+        <is>
+          <t>dbms</t>
+        </is>
+      </c>
+      <c r="N19" s="6" t="inlineStr">
+        <is>
+          <t>data st</t>
+        </is>
+      </c>
+      <c r="O19" s="6" t="inlineStr">
+        <is>
+          <t>Hive</t>
+        </is>
+      </c>
+      <c r="P19" s="6" t="inlineStr">
+        <is>
+          <t>pig</t>
+        </is>
+      </c>
+      <c r="Q19" s="6" t="inlineStr">
+        <is>
+          <t>sqoop</t>
+        </is>
+      </c>
+      <c r="R19" s="6" t="inlineStr">
+        <is>
+          <t>MapR</t>
+        </is>
+      </c>
+      <c r="S19" s="6" t="inlineStr">
+        <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="T19" s="6" t="inlineStr">
+        <is>
+          <t>GCP</t>
+        </is>
+      </c>
+      <c r="U19" s="6" t="inlineStr">
+        <is>
+          <t>Azure</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>99004352</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>Domain</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+      <c r="D20" s="6" t="inlineStr">
+        <is>
+          <t>QW</t>
+        </is>
+      </c>
+      <c r="E20" s="6" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="F20" s="6" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="G20" s="6" t="inlineStr">
+        <is>
+          <t>WQ</t>
+        </is>
+      </c>
+      <c r="H20" s="6" t="inlineStr">
+        <is>
+          <t>XS</t>
+        </is>
+      </c>
+      <c r="I20" s="6" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
+      <c r="J20" s="6" t="inlineStr">
+        <is>
+          <t>KI</t>
+        </is>
+      </c>
+      <c r="K20" s="6" t="inlineStr">
+        <is>
+          <t>KT</t>
+        </is>
+      </c>
+      <c r="L20" s="6" t="inlineStr">
+        <is>
+          <t>KA</t>
+        </is>
+      </c>
+      <c r="M20" s="6" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="N20" s="6" t="inlineStr">
+        <is>
+          <t>VF</t>
+        </is>
+      </c>
+      <c r="O20" s="6" t="inlineStr">
+        <is>
+          <t>OP</t>
+        </is>
+      </c>
+      <c r="P20" s="6" t="inlineStr">
+        <is>
+          <t>PW</t>
+        </is>
+      </c>
+      <c r="Q20" s="6" t="inlineStr">
+        <is>
+          <t>QI</t>
+        </is>
+      </c>
+      <c r="R20" s="6" t="inlineStr">
+        <is>
+          <t>OP</t>
+        </is>
+      </c>
+      <c r="S20" s="6" t="inlineStr">
+        <is>
+          <t>JH</t>
+        </is>
+      </c>
+      <c r="T20" s="6" t="inlineStr">
+        <is>
+          <t>FS</t>
+        </is>
+      </c>
+      <c r="U20" s="6" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>99004354</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>Hobbies</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>IGI</t>
+        </is>
+      </c>
+      <c r="D21" s="6" t="inlineStr">
+        <is>
+          <t>pubg</t>
+        </is>
+      </c>
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="F21" s="6" t="inlineStr">
+        <is>
+          <t>kabaddi</t>
+        </is>
+      </c>
+      <c r="G21" s="6" t="inlineStr">
+        <is>
+          <t>rugby</t>
+        </is>
+      </c>
+      <c r="H21" s="6" t="inlineStr">
+        <is>
+          <t>baseball</t>
+        </is>
+      </c>
+      <c r="I21" s="6" t="inlineStr">
+        <is>
+          <t>handball</t>
+        </is>
+      </c>
+      <c r="J21" s="6" t="inlineStr">
+        <is>
+          <t>sprint</t>
+        </is>
+      </c>
+      <c r="K21" s="6" t="inlineStr">
+        <is>
+          <t>lifting</t>
+        </is>
+      </c>
+      <c r="L21" s="6" t="inlineStr">
+        <is>
+          <t>shooting</t>
+        </is>
+      </c>
+      <c r="M21" s="6" t="inlineStr">
+        <is>
+          <t>GTA</t>
+        </is>
+      </c>
+      <c r="N21" s="6" t="inlineStr">
+        <is>
+          <t>baseball</t>
+        </is>
+      </c>
+      <c r="O21" s="6" t="inlineStr">
+        <is>
+          <t>handball</t>
+        </is>
+      </c>
+      <c r="P21" s="6" t="inlineStr">
+        <is>
+          <t>rugby</t>
+        </is>
+      </c>
+      <c r="Q21" s="6" t="inlineStr">
+        <is>
+          <t>baseball</t>
+        </is>
+      </c>
+      <c r="R21" s="6" t="inlineStr">
+        <is>
+          <t>pubg</t>
+        </is>
+      </c>
+      <c r="S21" s="6" t="inlineStr">
+        <is>
+          <t>COD</t>
+        </is>
+      </c>
+      <c r="T21" s="6" t="inlineStr">
+        <is>
+          <t>kabaddi</t>
+        </is>
+      </c>
+      <c r="U21" s="6" t="inlineStr">
+        <is>
+          <t>rugby</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>99004362</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Cities</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>hyderabad</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>bangalore</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>mumbai</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>chennai</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>indore</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>matura</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>shimla</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>jammu</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>indore</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>mangalore</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>kochi</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>kota</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>jaipur</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>shimla</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>jammu</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>cuttack</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>sambalpur</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>vijaywada</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>cuttack</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try catch block added new pylint score 9.11
</commit_message>
<xml_diff>
--- a/Implementation/Outputs.xlsx
+++ b/Implementation/Outputs.xlsx
@@ -484,7 +484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C301" activePane="bottomRight" state="frozen"/>
@@ -2319,109 +2319,323 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="6" t="inlineStr">
         <is>
           <t>99004362</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="6" t="inlineStr">
         <is>
           <t>Cities</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="6" t="inlineStr">
         <is>
           <t>hyderabad</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D22" s="6" t="inlineStr">
         <is>
           <t>bangalore</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E22" s="6" t="inlineStr">
         <is>
           <t>mumbai</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" s="6" t="inlineStr">
         <is>
           <t>chennai</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="G22" s="6" t="inlineStr">
         <is>
           <t>indore</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="H22" s="6" t="inlineStr">
         <is>
           <t>matura</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="I22" s="6" t="inlineStr">
         <is>
           <t>shimla</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="J22" s="6" t="inlineStr">
         <is>
           <t>jammu</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="K22" s="6" t="inlineStr">
         <is>
           <t>indore</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
+      <c r="L22" s="6" t="inlineStr">
         <is>
           <t>mangalore</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="M22" s="6" t="inlineStr">
         <is>
           <t>kochi</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr">
+      <c r="N22" s="6" t="inlineStr">
         <is>
           <t>kota</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr">
+      <c r="O22" s="6" t="inlineStr">
         <is>
           <t>jaipur</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr">
+      <c r="P22" s="6" t="inlineStr">
         <is>
           <t>shimla</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="Q22" s="6" t="inlineStr">
         <is>
           <t>jammu</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr">
+      <c r="R22" s="6" t="inlineStr">
         <is>
           <t>cuttack</t>
         </is>
       </c>
-      <c r="S22" t="inlineStr">
+      <c r="S22" s="6" t="inlineStr">
         <is>
           <t>sambalpur</t>
         </is>
       </c>
-      <c r="T22" t="inlineStr">
+      <c r="T22" s="6" t="inlineStr">
         <is>
           <t>vijaywada</t>
         </is>
       </c>
-      <c r="U22" t="inlineStr">
+      <c r="U22" s="6" t="inlineStr">
         <is>
           <t>cuttack</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>99004351</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>Domain</t>
+        </is>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D23" s="6" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E23" s="6" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="F23" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G23" s="6" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="H23" s="6" t="inlineStr">
+        <is>
+          <t>FG</t>
+        </is>
+      </c>
+      <c r="I23" s="6" t="inlineStr">
+        <is>
+          <t>WE</t>
+        </is>
+      </c>
+      <c r="J23" s="6" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="K23" s="6" t="inlineStr">
+        <is>
+          <t>SS</t>
+        </is>
+      </c>
+      <c r="L23" s="6" t="inlineStr">
+        <is>
+          <t>VF</t>
+        </is>
+      </c>
+      <c r="M23" s="6" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="N23" s="6" t="inlineStr">
+        <is>
+          <t>GT</t>
+        </is>
+      </c>
+      <c r="O23" s="6" t="inlineStr">
+        <is>
+          <t>FD</t>
+        </is>
+      </c>
+      <c r="P23" s="6" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="Q23" s="6" t="inlineStr">
+        <is>
+          <t>SW</t>
+        </is>
+      </c>
+      <c r="R23" s="6" t="inlineStr">
+        <is>
+          <t>AS</t>
+        </is>
+      </c>
+      <c r="S23" s="6" t="inlineStr">
+        <is>
+          <t>QW</t>
+        </is>
+      </c>
+      <c r="T23" s="6" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="U23" s="6" t="inlineStr">
+        <is>
+          <t>RE</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>99004351</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Hobbies</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>cricket</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>football</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>bowling</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>chess</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>travel</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>riding</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>racing</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>swim</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>games</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>video</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">photo </t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>kabaddi</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>rugby</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>baseball</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>handball</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>sprint</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>lifting</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>shooting</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>GTA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
pylinting modified along with readme
</commit_message>
<xml_diff>
--- a/Implementation/Outputs.xlsx
+++ b/Implementation/Outputs.xlsx
@@ -484,7 +484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C301" activePane="bottomRight" state="frozen"/>
@@ -2640,110 +2640,179 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="6" t="inlineStr">
         <is>
           <t>99004361</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="6" t="inlineStr">
         <is>
           <t>PL</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="6" t="inlineStr">
         <is>
           <t>spark</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" s="6" t="inlineStr">
         <is>
           <t>Hive</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E25" s="6" t="inlineStr">
         <is>
           <t>pig</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" s="6" t="inlineStr">
         <is>
           <t>sqoop</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" s="6" t="inlineStr">
         <is>
           <t>selenum</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="H25" s="6" t="inlineStr">
         <is>
           <t>hadoop</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" s="6" t="inlineStr">
         <is>
           <t>selenum</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="J25" s="6" t="inlineStr">
         <is>
           <t>hadoop</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="K25" s="6" t="inlineStr">
         <is>
           <t>spark</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
+      <c r="L25" s="6" t="inlineStr">
         <is>
           <t>python</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="M25" s="6" t="inlineStr">
         <is>
           <t>algorithm</t>
         </is>
       </c>
-      <c r="N25" t="inlineStr">
+      <c r="N25" s="6" t="inlineStr">
         <is>
           <t>dbms</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="O25" s="6" t="inlineStr">
         <is>
           <t>data st</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr">
+      <c r="P25" s="6" t="inlineStr">
         <is>
           <t>Hive</t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr">
+      <c r="Q25" s="6" t="inlineStr">
         <is>
           <t>pig</t>
         </is>
       </c>
-      <c r="R25" t="inlineStr">
+      <c r="R25" s="6" t="inlineStr">
         <is>
           <t>sqoop</t>
         </is>
       </c>
-      <c r="S25" t="inlineStr">
+      <c r="S25" s="6" t="inlineStr">
         <is>
           <t>MapR</t>
         </is>
       </c>
-      <c r="T25" t="inlineStr">
+      <c r="T25" s="6" t="inlineStr">
         <is>
           <t>GCP</t>
         </is>
       </c>
-      <c r="U25" t="inlineStr">
+      <c r="U25" s="6" t="inlineStr">
         <is>
           <t>Linux</t>
         </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>99004351</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Sem</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>93</v>
+      </c>
+      <c r="D26" t="n">
+        <v>52</v>
+      </c>
+      <c r="E26" t="n">
+        <v>65</v>
+      </c>
+      <c r="F26" t="n">
+        <v>39</v>
+      </c>
+      <c r="G26" t="n">
+        <v>87</v>
+      </c>
+      <c r="H26" t="n">
+        <v>43</v>
+      </c>
+      <c r="I26" t="n">
+        <v>55</v>
+      </c>
+      <c r="J26" t="n">
+        <v>65</v>
+      </c>
+      <c r="K26" t="n">
+        <v>99</v>
+      </c>
+      <c r="L26" t="n">
+        <v>91</v>
+      </c>
+      <c r="M26" t="n">
+        <v>64</v>
+      </c>
+      <c r="N26" t="n">
+        <v>75</v>
+      </c>
+      <c r="O26" t="n">
+        <v>79</v>
+      </c>
+      <c r="P26" t="n">
+        <v>86</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>44</v>
+      </c>
+      <c r="R26" t="n">
+        <v>75</v>
+      </c>
+      <c r="S26" t="n">
+        <v>98</v>
+      </c>
+      <c r="T26" t="n">
+        <v>23</v>
+      </c>
+      <c r="U26" t="n">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>